<commit_message>
powertrace AND BayesClassification AND vary windows
</commit_message>
<xml_diff>
--- a/results/powertrace/excel_files/powertrace_wind_5.xlsx
+++ b/results/powertrace/excel_files/powertrace_wind_5.xlsx
@@ -73,103 +73,103 @@
     <t xml:space="preserve">date</t>
   </si>
   <si>
-    <t xml:space="preserve">2018-08-13 13:50:16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:50:26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:50:36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:50:46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:50:56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:51:06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:51:16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:51:26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:51:36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:51:46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:51:56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:52:06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:52:16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:52:26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:52:36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:52:46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:52:56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:53:06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:53:16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:53:26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:53:36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:53:46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:53:56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:54:06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:54:16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:54:26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:54:36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:54:46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:54:56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:55:06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:55:16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:55:26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018-08-13 13:55:36</t>
+    <t xml:space="preserve">2018-08-14 12:17:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:17:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:17:21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:17:31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:17:41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:17:51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:18:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:18:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:18:21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:18:31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:18:41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:18:51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:19:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:19:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:19:21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:19:31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:19:41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:19:51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:20:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:20:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:20:21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:20:31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:20:41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:20:51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:21:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:21:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:21:21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:21:31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:21:41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:21:51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:22:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:22:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08-14 12:22:21</t>
   </si>
 </sst>
 </file>
@@ -353,28 +353,28 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>14155</v>
+        <v>6475</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>116911</v>
+        <v>55043</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>3487454</v>
+        <v>1583242</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>51881</v>
+        <v>21325</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>33167</v>
+        <v>13400</v>
       </c>
       <c r="I2" s="0" t="n">
         <v>0</v>
@@ -383,16 +383,16 @@
         <v>0</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>7387</v>
+        <v>11678</v>
       </c>
       <c r="L2" s="0" t="n">
-        <v>320293</v>
+        <v>316002</v>
       </c>
       <c r="M2" s="0" t="n">
-        <v>2908</v>
+        <v>6011</v>
       </c>
       <c r="N2" s="0" t="n">
-        <v>2375</v>
+        <v>3121</v>
       </c>
       <c r="O2" s="0" t="n">
         <v>0</v>
@@ -406,28 +406,28 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>15435</v>
+        <v>7755</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>128624</v>
+        <v>66726</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>3803421</v>
+        <v>1899239</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>58353</v>
+        <v>27596</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>36989</v>
+        <v>16677</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>0</v>
@@ -436,16 +436,16 @@
         <v>0</v>
       </c>
       <c r="K3" s="0" t="n">
-        <v>11713</v>
+        <v>11683</v>
       </c>
       <c r="L3" s="0" t="n">
-        <v>315967</v>
+        <v>315997</v>
       </c>
       <c r="M3" s="0" t="n">
-        <v>6472</v>
+        <v>6271</v>
       </c>
       <c r="N3" s="0" t="n">
-        <v>3822</v>
+        <v>3277</v>
       </c>
       <c r="O3" s="0" t="n">
         <v>0</v>
@@ -459,28 +459,28 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>16715</v>
+        <v>9035</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>136116</v>
+        <v>74051</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>4123609</v>
+        <v>2219594</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>61646</v>
+        <v>30505</v>
       </c>
       <c r="H4" s="0" t="n">
-        <v>39685</v>
+        <v>19141</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>0</v>
@@ -489,16 +489,16 @@
         <v>0</v>
       </c>
       <c r="K4" s="0" t="n">
-        <v>7492</v>
+        <v>7325</v>
       </c>
       <c r="L4" s="0" t="n">
-        <v>320188</v>
+        <v>320355</v>
       </c>
       <c r="M4" s="0" t="n">
-        <v>3293</v>
+        <v>2909</v>
       </c>
       <c r="N4" s="0" t="n">
-        <v>2696</v>
+        <v>2464</v>
       </c>
       <c r="O4" s="0" t="n">
         <v>0</v>
@@ -512,28 +512,28 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>17995</v>
+        <v>10315</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>147868</v>
+        <v>85984</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>4439537</v>
+        <v>2535341</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>67525</v>
+        <v>37160</v>
       </c>
       <c r="H5" s="0" t="n">
-        <v>42874</v>
+        <v>22464</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>0</v>
@@ -542,16 +542,16 @@
         <v>0</v>
       </c>
       <c r="K5" s="0" t="n">
-        <v>11752</v>
+        <v>11933</v>
       </c>
       <c r="L5" s="0" t="n">
-        <v>315928</v>
+        <v>315747</v>
       </c>
       <c r="M5" s="0" t="n">
-        <v>5879</v>
+        <v>6655</v>
       </c>
       <c r="N5" s="0" t="n">
-        <v>3189</v>
+        <v>3323</v>
       </c>
       <c r="O5" s="0" t="n">
         <v>0</v>
@@ -565,28 +565,28 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>19275</v>
+        <v>11595</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>155252</v>
+        <v>93340</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>4759833</v>
+        <v>2855665</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>70433</v>
+        <v>40068</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>45253</v>
+        <v>24720</v>
       </c>
       <c r="I6" s="0" t="n">
         <v>0</v>
@@ -595,16 +595,16 @@
         <v>0</v>
       </c>
       <c r="K6" s="0" t="n">
-        <v>7384</v>
+        <v>7356</v>
       </c>
       <c r="L6" s="0" t="n">
-        <v>320296</v>
+        <v>320324</v>
       </c>
       <c r="M6" s="0" t="n">
         <v>2908</v>
       </c>
       <c r="N6" s="0" t="n">
-        <v>2379</v>
+        <v>2256</v>
       </c>
       <c r="O6" s="0" t="n">
         <v>0</v>
@@ -618,28 +618,28 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>20570</v>
+        <v>12875</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>167066</v>
+        <v>105055</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>5079741</v>
+        <v>3171631</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>77082</v>
+        <v>46657</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>48787</v>
+        <v>28326</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>0</v>
@@ -648,16 +648,16 @@
         <v>0</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>11814</v>
+        <v>11715</v>
       </c>
       <c r="L7" s="0" t="n">
-        <v>319908</v>
+        <v>315966</v>
       </c>
       <c r="M7" s="0" t="n">
-        <v>6649</v>
+        <v>6589</v>
       </c>
       <c r="N7" s="0" t="n">
-        <v>3534</v>
+        <v>3606</v>
       </c>
       <c r="O7" s="0" t="n">
         <v>0</v>
@@ -671,28 +671,28 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>21835</v>
+        <v>14155</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>174502</v>
+        <v>112410</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>5395943</v>
+        <v>3491955</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>80442</v>
+        <v>50017</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>51478</v>
+        <v>30987</v>
       </c>
       <c r="I8" s="0" t="n">
         <v>0</v>
@@ -701,16 +701,16 @@
         <v>0</v>
       </c>
       <c r="K8" s="0" t="n">
-        <v>7436</v>
+        <v>7355</v>
       </c>
       <c r="L8" s="0" t="n">
-        <v>316202</v>
+        <v>320324</v>
       </c>
       <c r="M8" s="0" t="n">
         <v>3360</v>
       </c>
       <c r="N8" s="0" t="n">
-        <v>2691</v>
+        <v>2661</v>
       </c>
       <c r="O8" s="0" t="n">
         <v>0</v>
@@ -724,28 +724,28 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>23115</v>
+        <v>15435</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>186256</v>
+        <v>124264</v>
       </c>
       <c r="F9" s="0" t="n">
-        <v>5711869</v>
+        <v>3807781</v>
       </c>
       <c r="G9" s="0" t="n">
-        <v>86648</v>
+        <v>56281</v>
       </c>
       <c r="H9" s="0" t="n">
-        <v>54535</v>
+        <v>34477</v>
       </c>
       <c r="I9" s="0" t="n">
         <v>0</v>
@@ -754,16 +754,16 @@
         <v>0</v>
       </c>
       <c r="K9" s="0" t="n">
-        <v>11754</v>
+        <v>11854</v>
       </c>
       <c r="L9" s="0" t="n">
-        <v>315926</v>
+        <v>315826</v>
       </c>
       <c r="M9" s="0" t="n">
-        <v>6206</v>
+        <v>6264</v>
       </c>
       <c r="N9" s="0" t="n">
-        <v>3057</v>
+        <v>3490</v>
       </c>
       <c r="O9" s="0" t="n">
         <v>0</v>
@@ -777,28 +777,28 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>24395</v>
+        <v>16715</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>193600</v>
+        <v>136019</v>
       </c>
       <c r="F10" s="0" t="n">
-        <v>6032205</v>
+        <v>4123685</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>89557</v>
+        <v>62545</v>
       </c>
       <c r="H10" s="0" t="n">
-        <v>57191</v>
+        <v>37786</v>
       </c>
       <c r="I10" s="0" t="n">
         <v>0</v>
@@ -807,16 +807,16 @@
         <v>0</v>
       </c>
       <c r="K10" s="0" t="n">
-        <v>7344</v>
+        <v>11754</v>
       </c>
       <c r="L10" s="0" t="n">
-        <v>320336</v>
+        <v>315904</v>
       </c>
       <c r="M10" s="0" t="n">
-        <v>2909</v>
+        <v>6264</v>
       </c>
       <c r="N10" s="0" t="n">
-        <v>2656</v>
+        <v>3309</v>
       </c>
       <c r="O10" s="0" t="n">
         <v>0</v>
@@ -830,28 +830,28 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>25675</v>
+        <v>17995</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>205400</v>
+        <v>143448</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>6348085</v>
+        <v>4443957</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>96211</v>
+        <v>65839</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>60931</v>
+        <v>40405</v>
       </c>
       <c r="I11" s="0" t="n">
         <v>0</v>
@@ -860,16 +860,16 @@
         <v>0</v>
       </c>
       <c r="K11" s="0" t="n">
-        <v>11800</v>
+        <v>7428</v>
       </c>
       <c r="L11" s="0" t="n">
-        <v>315880</v>
+        <v>320272</v>
       </c>
       <c r="M11" s="0" t="n">
-        <v>6654</v>
+        <v>3294</v>
       </c>
       <c r="N11" s="0" t="n">
-        <v>3740</v>
+        <v>2619</v>
       </c>
       <c r="O11" s="0" t="n">
         <v>0</v>
@@ -883,28 +883,28 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>26955</v>
+        <v>19275</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>217112</v>
+        <v>155104</v>
       </c>
       <c r="F12" s="0" t="n">
-        <v>6664053</v>
+        <v>4759981</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>102550</v>
+        <v>72107</v>
       </c>
       <c r="H12" s="0" t="n">
-        <v>64233</v>
+        <v>43837</v>
       </c>
       <c r="I12" s="0" t="n">
         <v>0</v>
@@ -913,16 +913,16 @@
         <v>0</v>
       </c>
       <c r="K12" s="0" t="n">
-        <v>11712</v>
+        <v>11656</v>
       </c>
       <c r="L12" s="0" t="n">
-        <v>315968</v>
+        <v>316024</v>
       </c>
       <c r="M12" s="0" t="n">
-        <v>6339</v>
+        <v>6268</v>
       </c>
       <c r="N12" s="0" t="n">
-        <v>3302</v>
+        <v>3432</v>
       </c>
       <c r="O12" s="0" t="n">
         <v>0</v>
@@ -936,28 +936,28 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>28235</v>
+        <v>20555</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>228872</v>
+        <v>166842</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>6979973</v>
+        <v>5075902</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>108815</v>
+        <v>78571</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>67523</v>
+        <v>47121</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>0</v>
@@ -966,16 +966,16 @@
         <v>0</v>
       </c>
       <c r="K13" s="0" t="n">
-        <v>11760</v>
+        <v>11738</v>
       </c>
       <c r="L13" s="0" t="n">
-        <v>315920</v>
+        <v>315921</v>
       </c>
       <c r="M13" s="0" t="n">
-        <v>6265</v>
+        <v>6464</v>
       </c>
       <c r="N13" s="0" t="n">
-        <v>3290</v>
+        <v>3284</v>
       </c>
       <c r="O13" s="0" t="n">
         <v>0</v>
@@ -989,28 +989,28 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>29515</v>
+        <v>21835</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>240609</v>
+        <v>174237</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>7295916</v>
+        <v>5396208</v>
       </c>
       <c r="G14" s="0" t="n">
-        <v>114631</v>
+        <v>81993</v>
       </c>
       <c r="H14" s="0" t="n">
-        <v>70485</v>
+        <v>49833</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>0</v>
@@ -1019,16 +1019,16 @@
         <v>0</v>
       </c>
       <c r="K14" s="0" t="n">
-        <v>11737</v>
+        <v>7394</v>
       </c>
       <c r="L14" s="0" t="n">
-        <v>315943</v>
+        <v>320306</v>
       </c>
       <c r="M14" s="0" t="n">
-        <v>5816</v>
+        <v>3422</v>
       </c>
       <c r="N14" s="0" t="n">
-        <v>2962</v>
+        <v>2712</v>
       </c>
       <c r="O14" s="0" t="n">
         <v>0</v>
@@ -1042,28 +1042,28 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>30811</v>
+        <v>23115</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>252504</v>
+        <v>186033</v>
       </c>
       <c r="F15" s="0" t="n">
-        <v>7616023</v>
+        <v>5712092</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>120837</v>
+        <v>87810</v>
       </c>
       <c r="H15" s="0" t="n">
-        <v>73832</v>
+        <v>52931</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>0</v>
@@ -1072,16 +1072,16 @@
         <v>0</v>
       </c>
       <c r="K15" s="0" t="n">
-        <v>11895</v>
+        <v>11796</v>
       </c>
       <c r="L15" s="0" t="n">
-        <v>320107</v>
+        <v>315884</v>
       </c>
       <c r="M15" s="0" t="n">
-        <v>6206</v>
+        <v>5817</v>
       </c>
       <c r="N15" s="0" t="n">
-        <v>3347</v>
+        <v>3098</v>
       </c>
       <c r="O15" s="0" t="n">
         <v>0</v>
@@ -1095,28 +1095,28 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>32075</v>
+        <v>24395</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>264186</v>
+        <v>193390</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>7927699</v>
+        <v>6032415</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>126917</v>
+        <v>90718</v>
       </c>
       <c r="H16" s="0" t="n">
-        <v>77257</v>
+        <v>55408</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>0</v>
@@ -1125,16 +1125,16 @@
         <v>0</v>
       </c>
       <c r="K16" s="0" t="n">
-        <v>11682</v>
+        <v>7357</v>
       </c>
       <c r="L16" s="0" t="n">
-        <v>311676</v>
+        <v>320323</v>
       </c>
       <c r="M16" s="0" t="n">
-        <v>6080</v>
+        <v>2908</v>
       </c>
       <c r="N16" s="0" t="n">
-        <v>3425</v>
+        <v>2477</v>
       </c>
       <c r="O16" s="0" t="n">
         <v>0</v>
@@ -1148,28 +1148,28 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>33355</v>
+        <v>25675</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>271598</v>
+        <v>205039</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>8247967</v>
+        <v>6348446</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>130145</v>
+        <v>96534</v>
       </c>
       <c r="H17" s="0" t="n">
-        <v>79906</v>
+        <v>58614</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>0</v>
@@ -1178,16 +1178,16 @@
         <v>0</v>
       </c>
       <c r="K17" s="0" t="n">
-        <v>7412</v>
+        <v>11649</v>
       </c>
       <c r="L17" s="0" t="n">
-        <v>320268</v>
+        <v>316031</v>
       </c>
       <c r="M17" s="0" t="n">
-        <v>3228</v>
+        <v>5816</v>
       </c>
       <c r="N17" s="0" t="n">
-        <v>2649</v>
+        <v>3206</v>
       </c>
       <c r="O17" s="0" t="n">
         <v>0</v>
@@ -1201,28 +1201,28 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>34635</v>
+        <v>26955</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>283474</v>
+        <v>216696</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>8563771</v>
+        <v>6664469</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>136476</v>
+        <v>102352</v>
       </c>
       <c r="H18" s="0" t="n">
-        <v>83137</v>
+        <v>61659</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>0</v>
@@ -1231,16 +1231,16 @@
         <v>0</v>
       </c>
       <c r="K18" s="0" t="n">
-        <v>11876</v>
+        <v>11657</v>
       </c>
       <c r="L18" s="0" t="n">
-        <v>315804</v>
+        <v>316023</v>
       </c>
       <c r="M18" s="0" t="n">
-        <v>6331</v>
+        <v>5818</v>
       </c>
       <c r="N18" s="0" t="n">
-        <v>3231</v>
+        <v>3045</v>
       </c>
       <c r="O18" s="0" t="n">
         <v>0</v>
@@ -1254,28 +1254,28 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>35915</v>
+        <v>28235</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D19" s="0" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>290962</v>
+        <v>224057</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>8883963</v>
+        <v>6984788</v>
       </c>
       <c r="G19" s="0" t="n">
-        <v>139582</v>
+        <v>105456</v>
       </c>
       <c r="H19" s="0" t="n">
-        <v>86294</v>
+        <v>64219</v>
       </c>
       <c r="I19" s="0" t="n">
         <v>0</v>
@@ -1284,16 +1284,16 @@
         <v>0</v>
       </c>
       <c r="K19" s="0" t="n">
-        <v>7488</v>
+        <v>7361</v>
       </c>
       <c r="L19" s="0" t="n">
-        <v>320192</v>
+        <v>320319</v>
       </c>
       <c r="M19" s="0" t="n">
-        <v>3106</v>
+        <v>3104</v>
       </c>
       <c r="N19" s="0" t="n">
-        <v>3157</v>
+        <v>2560</v>
       </c>
       <c r="O19" s="0" t="n">
         <v>0</v>
@@ -1307,28 +1307,28 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="B20" s="0" t="n">
-        <v>37195</v>
+        <v>29515</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>302690</v>
+        <v>235791</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>9199915</v>
+        <v>7300734</v>
       </c>
       <c r="G20" s="0" t="n">
-        <v>145655</v>
+        <v>111398</v>
       </c>
       <c r="H20" s="0" t="n">
-        <v>89771</v>
+        <v>67216</v>
       </c>
       <c r="I20" s="0" t="n">
         <v>0</v>
@@ -1337,16 +1337,16 @@
         <v>0</v>
       </c>
       <c r="K20" s="0" t="n">
-        <v>11727</v>
+        <v>11733</v>
       </c>
       <c r="L20" s="0" t="n">
-        <v>315952</v>
+        <v>315946</v>
       </c>
       <c r="M20" s="0" t="n">
-        <v>6073</v>
+        <v>5942</v>
       </c>
       <c r="N20" s="0" t="n">
-        <v>3477</v>
+        <v>2997</v>
       </c>
       <c r="O20" s="0" t="n">
         <v>0</v>
@@ -1360,28 +1360,28 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="B21" s="0" t="n">
-        <v>38475</v>
+        <v>30795</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>314410</v>
+        <v>247462</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>9515875</v>
+        <v>7616743</v>
       </c>
       <c r="G21" s="0" t="n">
-        <v>151797</v>
+        <v>117214</v>
       </c>
       <c r="H21" s="0" t="n">
-        <v>92951</v>
+        <v>70258</v>
       </c>
       <c r="I21" s="0" t="n">
         <v>0</v>
@@ -1390,16 +1390,16 @@
         <v>0</v>
       </c>
       <c r="K21" s="0" t="n">
-        <v>11720</v>
+        <v>11671</v>
       </c>
       <c r="L21" s="0" t="n">
-        <v>315960</v>
+        <v>316009</v>
       </c>
       <c r="M21" s="0" t="n">
-        <v>6142</v>
+        <v>5816</v>
       </c>
       <c r="N21" s="0" t="n">
-        <v>3180</v>
+        <v>3042</v>
       </c>
       <c r="O21" s="0" t="n">
         <v>0</v>
@@ -1413,28 +1413,28 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>39755</v>
+        <v>32075</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>321813</v>
+        <v>254838</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>9836152</v>
+        <v>7937047</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>154708</v>
+        <v>120508</v>
       </c>
       <c r="H22" s="0" t="n">
-        <v>95469</v>
+        <v>72776</v>
       </c>
       <c r="I22" s="0" t="n">
         <v>0</v>
@@ -1443,13 +1443,13 @@
         <v>0</v>
       </c>
       <c r="K22" s="0" t="n">
-        <v>7403</v>
+        <v>7376</v>
       </c>
       <c r="L22" s="0" t="n">
-        <v>320277</v>
+        <v>320304</v>
       </c>
       <c r="M22" s="0" t="n">
-        <v>2911</v>
+        <v>3294</v>
       </c>
       <c r="N22" s="0" t="n">
         <v>2518</v>
@@ -1466,28 +1466,28 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>41035</v>
+        <v>33355</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E23" s="0" t="n">
-        <v>333562</v>
+        <v>266580</v>
       </c>
       <c r="F23" s="0" t="n">
-        <v>10152083</v>
+        <v>8252985</v>
       </c>
       <c r="G23" s="0" t="n">
-        <v>160720</v>
+        <v>126452</v>
       </c>
       <c r="H23" s="0" t="n">
-        <v>98517</v>
+        <v>75785</v>
       </c>
       <c r="I23" s="0" t="n">
         <v>0</v>
@@ -1496,16 +1496,16 @@
         <v>0</v>
       </c>
       <c r="K23" s="0" t="n">
-        <v>11749</v>
+        <v>11742</v>
       </c>
       <c r="L23" s="0" t="n">
-        <v>315931</v>
+        <v>315938</v>
       </c>
       <c r="M23" s="0" t="n">
-        <v>6012</v>
+        <v>5944</v>
       </c>
       <c r="N23" s="0" t="n">
-        <v>3048</v>
+        <v>3009</v>
       </c>
       <c r="O23" s="0" t="n">
         <v>0</v>
@@ -1519,28 +1519,28 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="B24" s="0" t="n">
-        <v>42315</v>
+        <v>34635</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D24" s="0" t="n">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E24" s="0" t="n">
-        <v>341038</v>
+        <v>278310</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>10472287</v>
+        <v>8568914</v>
       </c>
       <c r="G24" s="0" t="n">
-        <v>163695</v>
+        <v>132982</v>
       </c>
       <c r="H24" s="0" t="n">
-        <v>101440</v>
+        <v>79303</v>
       </c>
       <c r="I24" s="0" t="n">
         <v>0</v>
@@ -1549,16 +1549,16 @@
         <v>0</v>
       </c>
       <c r="K24" s="0" t="n">
-        <v>7476</v>
+        <v>11730</v>
       </c>
       <c r="L24" s="0" t="n">
-        <v>320204</v>
+        <v>315929</v>
       </c>
       <c r="M24" s="0" t="n">
-        <v>2975</v>
+        <v>6530</v>
       </c>
       <c r="N24" s="0" t="n">
-        <v>2923</v>
+        <v>3518</v>
       </c>
       <c r="O24" s="0" t="n">
         <v>0</v>
@@ -1572,28 +1572,28 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B25" s="0" t="n">
-        <v>43595</v>
+        <v>35915</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D25" s="0" t="n">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E25" s="0" t="n">
-        <v>352757</v>
+        <v>285708</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>10788248</v>
+        <v>8889217</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>169512</v>
+        <v>136080</v>
       </c>
       <c r="H25" s="0" t="n">
-        <v>104396</v>
+        <v>81737</v>
       </c>
       <c r="I25" s="0" t="n">
         <v>0</v>
@@ -1602,16 +1602,16 @@
         <v>0</v>
       </c>
       <c r="K25" s="0" t="n">
-        <v>11719</v>
+        <v>7397</v>
       </c>
       <c r="L25" s="0" t="n">
-        <v>315961</v>
+        <v>320303</v>
       </c>
       <c r="M25" s="0" t="n">
-        <v>5817</v>
+        <v>3098</v>
       </c>
       <c r="N25" s="0" t="n">
-        <v>2956</v>
+        <v>2434</v>
       </c>
       <c r="O25" s="0" t="n">
         <v>0</v>
@@ -1625,28 +1625,28 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="B26" s="0" t="n">
-        <v>44875</v>
+        <v>37195</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>364513</v>
+        <v>297417</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>11104172</v>
+        <v>9205188</v>
       </c>
       <c r="G26" s="0" t="n">
-        <v>175719</v>
+        <v>142220</v>
       </c>
       <c r="H26" s="0" t="n">
-        <v>107776</v>
+        <v>84751</v>
       </c>
       <c r="I26" s="0" t="n">
         <v>0</v>
@@ -1655,16 +1655,16 @@
         <v>0</v>
       </c>
       <c r="K26" s="0" t="n">
-        <v>11756</v>
+        <v>11709</v>
       </c>
       <c r="L26" s="0" t="n">
-        <v>315924</v>
+        <v>315971</v>
       </c>
       <c r="M26" s="0" t="n">
-        <v>6207</v>
+        <v>6140</v>
       </c>
       <c r="N26" s="0" t="n">
-        <v>3380</v>
+        <v>3014</v>
       </c>
       <c r="O26" s="0" t="n">
         <v>0</v>
@@ -1678,28 +1678,28 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="B27" s="0" t="n">
-        <v>46170</v>
+        <v>38475</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>371874</v>
+        <v>304793</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>11428533</v>
+        <v>9525492</v>
       </c>
       <c r="G27" s="0" t="n">
-        <v>178823</v>
+        <v>145192</v>
       </c>
       <c r="H27" s="0" t="n">
-        <v>110528</v>
+        <v>87134</v>
       </c>
       <c r="I27" s="0" t="n">
         <v>0</v>
@@ -1708,16 +1708,16 @@
         <v>0</v>
       </c>
       <c r="K27" s="0" t="n">
-        <v>7361</v>
+        <v>7375</v>
       </c>
       <c r="L27" s="0" t="n">
-        <v>324361</v>
+        <v>320304</v>
       </c>
       <c r="M27" s="0" t="n">
-        <v>3104</v>
+        <v>2972</v>
       </c>
       <c r="N27" s="0" t="n">
-        <v>2752</v>
+        <v>2383</v>
       </c>
       <c r="O27" s="0" t="n">
         <v>0</v>
@@ -1731,28 +1731,28 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="B28" s="0" t="n">
-        <v>47435</v>
+        <v>39755</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>383500</v>
+        <v>316500</v>
       </c>
       <c r="F28" s="0" t="n">
-        <v>11740780</v>
+        <v>9841465</v>
       </c>
       <c r="G28" s="0" t="n">
-        <v>184639</v>
+        <v>151394</v>
       </c>
       <c r="H28" s="0" t="n">
-        <v>114241</v>
+        <v>90368</v>
       </c>
       <c r="I28" s="0" t="n">
         <v>0</v>
@@ -1761,16 +1761,16 @@
         <v>0</v>
       </c>
       <c r="K28" s="0" t="n">
-        <v>11626</v>
+        <v>11707</v>
       </c>
       <c r="L28" s="0" t="n">
-        <v>312247</v>
+        <v>315973</v>
       </c>
       <c r="M28" s="0" t="n">
-        <v>5816</v>
+        <v>6202</v>
       </c>
       <c r="N28" s="0" t="n">
-        <v>3713</v>
+        <v>3234</v>
       </c>
       <c r="O28" s="0" t="n">
         <v>0</v>
@@ -1784,28 +1784,28 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="B29" s="0" t="n">
-        <v>48715</v>
+        <v>41035</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>391043</v>
+        <v>328220</v>
       </c>
       <c r="F29" s="0" t="n">
-        <v>12060682</v>
+        <v>10157404</v>
       </c>
       <c r="G29" s="0" t="n">
-        <v>187548</v>
+        <v>157917</v>
       </c>
       <c r="H29" s="0" t="n">
-        <v>116688</v>
+        <v>93936</v>
       </c>
       <c r="I29" s="0" t="n">
         <v>0</v>
@@ -1814,16 +1814,16 @@
         <v>0</v>
       </c>
       <c r="K29" s="0" t="n">
-        <v>7542</v>
+        <v>11720</v>
       </c>
       <c r="L29" s="0" t="n">
-        <v>319902</v>
+        <v>315939</v>
       </c>
       <c r="M29" s="0" t="n">
-        <v>2909</v>
+        <v>6523</v>
       </c>
       <c r="N29" s="0" t="n">
-        <v>2447</v>
+        <v>3568</v>
       </c>
       <c r="O29" s="0" t="n">
         <v>0</v>
@@ -1837,28 +1837,28 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="B30" s="0" t="n">
-        <v>49995</v>
+        <v>42315</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>398408</v>
+        <v>335706</v>
       </c>
       <c r="F30" s="0" t="n">
-        <v>12380997</v>
+        <v>10477619</v>
       </c>
       <c r="G30" s="0" t="n">
-        <v>190716</v>
+        <v>160826</v>
       </c>
       <c r="H30" s="0" t="n">
-        <v>119381</v>
+        <v>96241</v>
       </c>
       <c r="I30" s="0" t="n">
         <v>0</v>
@@ -1867,16 +1867,16 @@
         <v>0</v>
       </c>
       <c r="K30" s="0" t="n">
-        <v>7365</v>
+        <v>7485</v>
       </c>
       <c r="L30" s="0" t="n">
-        <v>320315</v>
+        <v>320215</v>
       </c>
       <c r="M30" s="0" t="n">
-        <v>3168</v>
+        <v>2909</v>
       </c>
       <c r="N30" s="0" t="n">
-        <v>2693</v>
+        <v>2305</v>
       </c>
       <c r="O30" s="0" t="n">
         <v>0</v>
@@ -1890,28 +1890,28 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="B31" s="0" t="n">
-        <v>51275</v>
+        <v>43595</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>410190</v>
+        <v>347545</v>
       </c>
       <c r="F31" s="0" t="n">
-        <v>12696895</v>
+        <v>10793460</v>
       </c>
       <c r="G31" s="0" t="n">
-        <v>197046</v>
+        <v>166708</v>
       </c>
       <c r="H31" s="0" t="n">
-        <v>122656</v>
+        <v>99184</v>
       </c>
       <c r="I31" s="0" t="n">
         <v>0</v>
@@ -1920,16 +1920,16 @@
         <v>0</v>
       </c>
       <c r="K31" s="0" t="n">
-        <v>11782</v>
+        <v>11839</v>
       </c>
       <c r="L31" s="0" t="n">
-        <v>315898</v>
+        <v>315841</v>
       </c>
       <c r="M31" s="0" t="n">
-        <v>6330</v>
+        <v>5882</v>
       </c>
       <c r="N31" s="0" t="n">
-        <v>3275</v>
+        <v>2943</v>
       </c>
       <c r="O31" s="0" t="n">
         <v>0</v>
@@ -1943,28 +1943,28 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>31</v>
+        <v>64</v>
       </c>
       <c r="B32" s="0" t="n">
-        <v>52555</v>
+        <v>44875</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>417682</v>
+        <v>354947</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>13017083</v>
+        <v>11113738</v>
       </c>
       <c r="G32" s="0" t="n">
-        <v>200211</v>
+        <v>169679</v>
       </c>
       <c r="H32" s="0" t="n">
-        <v>125548</v>
+        <v>101576</v>
       </c>
       <c r="I32" s="0" t="n">
         <v>0</v>
@@ -1973,16 +1973,16 @@
         <v>0</v>
       </c>
       <c r="K32" s="0" t="n">
-        <v>7492</v>
+        <v>7402</v>
       </c>
       <c r="L32" s="0" t="n">
-        <v>320188</v>
+        <v>320278</v>
       </c>
       <c r="M32" s="0" t="n">
-        <v>3165</v>
+        <v>2971</v>
       </c>
       <c r="N32" s="0" t="n">
-        <v>2892</v>
+        <v>2392</v>
       </c>
       <c r="O32" s="0" t="n">
         <v>0</v>
@@ -1996,28 +1996,28 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="B33" s="0" t="n">
-        <v>53835</v>
+        <v>46155</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E33" s="0" t="n">
-        <v>429408</v>
+        <v>366695</v>
       </c>
       <c r="F33" s="0" t="n">
-        <v>13333037</v>
+        <v>11429649</v>
       </c>
       <c r="G33" s="0" t="n">
-        <v>206347</v>
+        <v>176074</v>
       </c>
       <c r="H33" s="0" t="n">
-        <v>128859</v>
+        <v>104777</v>
       </c>
       <c r="I33" s="0" t="n">
         <v>0</v>
@@ -2026,16 +2026,16 @@
         <v>0</v>
       </c>
       <c r="K33" s="0" t="n">
-        <v>11726</v>
+        <v>11748</v>
       </c>
       <c r="L33" s="0" t="n">
-        <v>315954</v>
+        <v>315911</v>
       </c>
       <c r="M33" s="0" t="n">
-        <v>6136</v>
+        <v>6395</v>
       </c>
       <c r="N33" s="0" t="n">
-        <v>3311</v>
+        <v>3201</v>
       </c>
       <c r="O33" s="0" t="n">
         <v>0</v>
@@ -2049,28 +2049,28 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="B34" s="0" t="n">
-        <v>55115</v>
+        <v>47435</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E34" s="0" t="n">
-        <v>441221</v>
+        <v>374067</v>
       </c>
       <c r="F34" s="0" t="n">
-        <v>13648904</v>
+        <v>11749978</v>
       </c>
       <c r="G34" s="0" t="n">
-        <v>212679</v>
+        <v>178982</v>
       </c>
       <c r="H34" s="0" t="n">
-        <v>132111</v>
+        <v>107143</v>
       </c>
       <c r="I34" s="0" t="n">
         <v>0</v>
@@ -2079,16 +2079,16 @@
         <v>0</v>
       </c>
       <c r="K34" s="0" t="n">
-        <v>11813</v>
+        <v>7371</v>
       </c>
       <c r="L34" s="0" t="n">
-        <v>315867</v>
+        <v>320329</v>
       </c>
       <c r="M34" s="0" t="n">
-        <v>6332</v>
+        <v>2908</v>
       </c>
       <c r="N34" s="0" t="n">
-        <v>3252</v>
+        <v>2366</v>
       </c>
       <c r="O34" s="0" t="n">
         <v>0</v>

</xml_diff>